<commit_message>
Update Artefakte Open Space
</commit_message>
<xml_diff>
--- a/Artefakte/WS2122_ChouliarasBurgdorfWolf_PoC_Kriterien.xlsx
+++ b/Artefakte/WS2122_ChouliarasBurgdorfWolf_PoC_Kriterien.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Entwicklungsprojekt\EPW2122ChouliarasBurgdorfWolf\Artefakte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54646E07-3387-4A09-BEBA-023C323286BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A54492-9739-4720-967E-7CCD5BC07D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Kriterien PoC" sheetId="2" r:id="rId2"/>
-    <sheet name="Installationsbeschreibung" sheetId="3" r:id="rId3"/>
+    <sheet name="andere PoCs" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="70">
   <si>
     <t>Success</t>
   </si>
@@ -113,12 +113,6 @@
     <t>schnelles Aufsetzen ist KEIN Kriterium mehr,</t>
   </si>
   <si>
-    <t>Flutter</t>
-  </si>
-  <si>
-    <t>ThreeJS</t>
-  </si>
-  <si>
     <t>Kriterium</t>
   </si>
   <si>
@@ -272,7 +266,10 @@
     <t>Bei der Arbeit mit Three.JS konnten PoC's mit angemessenem Aufwand durchgeführt werden.</t>
   </si>
   <si>
-    <t>Unity</t>
+    <t>Routen Algorithmus</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
@@ -419,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -442,44 +439,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -886,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA11787-3E16-4845-B675-31D754FB2842}">
   <dimension ref="B1:AA16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="77" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q4:R11"/>
+    <sheetView zoomScale="77" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,23 +908,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="E1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="9"/>
-      <c r="I1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="8"/>
+      <c r="B1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="E1" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="I1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="18"/>
       <c r="K1" s="6"/>
-      <c r="P1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q1" s="8"/>
+      <c r="P1" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="18"/>
       <c r="R1" s="6"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.25">
@@ -941,298 +935,298 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="AA2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="T4" s="17"/>
+    </row>
+    <row r="5" spans="2:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="T5" s="17"/>
+    </row>
+    <row r="6" spans="2:27" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="R6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="S6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="T6" s="17"/>
+    </row>
+    <row r="7" spans="2:27" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="R7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="T7" s="17"/>
+    </row>
+    <row r="8" spans="2:27" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="P8" s="16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="2:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="2:27" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="P4" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="T4" s="23"/>
-    </row>
-    <row r="5" spans="2:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="17" t="s">
+      <c r="Q8" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="S8" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="T8" s="17"/>
+    </row>
+    <row r="9" spans="2:27" ht="63" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="P5" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q5" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="R5" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="S5" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="T5" s="23"/>
-    </row>
-    <row r="6" spans="2:27" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="S6" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="T6" s="23"/>
-    </row>
-    <row r="7" spans="2:27" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="M7" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="P7" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q7" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="R7" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="S7" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="T7" s="23"/>
-    </row>
-    <row r="8" spans="2:27" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="M8" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="P8" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q8" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="R8" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="S8" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="T8" s="23"/>
-    </row>
-    <row r="9" spans="2:27" ht="63" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -1244,20 +1238,20 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="2:27" ht="63" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>58</v>
+      <c r="B10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="I10" s="7" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">I9:L10</f>
@@ -1268,20 +1262,20 @@
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="2:27" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>64</v>
+      <c r="B11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -1305,120 +1299,142 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A38124-0217-4829-9A06-DB0D97D65209}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5EE435-9524-4D5A-BEB4-5EBAA1BB63EA}">
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="8" max="8" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="13"/>
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="6"/>
+      <c r="H1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="18"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="K3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>